<commit_message>
Clean up audio & image files
</commit_message>
<xml_diff>
--- a/material-vn/item_order.xlsx
+++ b/material-vn/item_order.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bohn/Research/QuantEx/orev-vn/material-vn/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliaprein/academiccloudsync/studies/orev-vn/material-vn/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E55F578E-27B6-7A46-A117-0CC2093A630F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB598A4-DCCC-C244-BC5C-16C902E67FA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32100" yWindow="960" windowWidth="27840" windowHeight="16740" xr2:uid="{9D79C90C-9F7D-2F46-9E4F-8B298AB5B9D9}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{9D79C90C-9F7D-2F46-9E4F-8B298AB5B9D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -41,15 +41,6 @@
     <t>target_de</t>
   </si>
   <si>
-    <t>phonological_distractor_de</t>
-  </si>
-  <si>
-    <t>semantic_distractor_de</t>
-  </si>
-  <si>
-    <t>unrelated_distractor_de</t>
-  </si>
-  <si>
     <t>schweben</t>
   </si>
   <si>
@@ -291,6 +282,15 @@
   </si>
   <si>
     <t>Audio</t>
+  </si>
+  <si>
+    <t>dist1_semantic_distractor_de</t>
+  </si>
+  <si>
+    <t>dist2_phonological_distractor_de</t>
+  </si>
+  <si>
+    <t>dist3_unrelated_distractor_de</t>
   </si>
 </sst>
 </file>
@@ -338,7 +338,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -354,7 +354,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -672,41 +672,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{799C0DEA-28D9-6C42-8CEC-3504E277A21A}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H21"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.33203125" customWidth="1"/>
     <col min="2" max="2" width="13.6640625" customWidth="1"/>
-    <col min="3" max="3" width="24.6640625" customWidth="1"/>
-    <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="24.1640625" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>83</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>84</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -714,16 +714,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
       </c>
       <c r="F2">
         <v>3</v>
@@ -737,16 +737,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -760,16 +760,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
         <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -783,16 +783,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
         <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" t="s">
-        <v>19</v>
       </c>
       <c r="F5">
         <v>4</v>
@@ -806,16 +806,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s">
         <v>20</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" t="s">
-        <v>23</v>
       </c>
       <c r="F6">
         <v>3</v>
@@ -829,16 +829,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s">
         <v>24</v>
-      </c>
-      <c r="C7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" t="s">
-        <v>27</v>
       </c>
       <c r="F7">
         <v>4</v>
@@ -852,16 +852,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" t="s">
         <v>28</v>
-      </c>
-      <c r="C8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" t="s">
-        <v>31</v>
       </c>
       <c r="F8">
         <v>2</v>
@@ -875,16 +875,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" t="s">
         <v>32</v>
-      </c>
-      <c r="C9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" t="s">
-        <v>35</v>
       </c>
       <c r="F9">
         <v>2</v>
@@ -898,16 +898,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" t="s">
         <v>36</v>
-      </c>
-      <c r="C10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" t="s">
-        <v>39</v>
       </c>
       <c r="F10">
         <v>4</v>
@@ -921,16 +921,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" t="s">
         <v>40</v>
-      </c>
-      <c r="C11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E11" t="s">
-        <v>43</v>
       </c>
       <c r="F11">
         <v>1</v>
@@ -944,16 +944,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="E12" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -967,16 +967,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" t="s">
         <v>47</v>
-      </c>
-      <c r="C13" t="s">
-        <v>48</v>
-      </c>
-      <c r="D13" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" t="s">
-        <v>50</v>
       </c>
       <c r="F13">
         <v>3</v>
@@ -990,16 +990,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" t="s">
         <v>51</v>
-      </c>
-      <c r="C14" t="s">
-        <v>52</v>
-      </c>
-      <c r="D14" t="s">
-        <v>53</v>
-      </c>
-      <c r="E14" t="s">
-        <v>54</v>
       </c>
       <c r="F14">
         <v>2</v>
@@ -1013,16 +1013,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" t="s">
         <v>55</v>
-      </c>
-      <c r="C15" t="s">
-        <v>56</v>
-      </c>
-      <c r="D15" t="s">
-        <v>57</v>
-      </c>
-      <c r="E15" t="s">
-        <v>58</v>
       </c>
       <c r="F15">
         <v>1</v>
@@ -1036,16 +1036,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" t="s">
         <v>59</v>
-      </c>
-      <c r="C16" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16" t="s">
-        <v>61</v>
-      </c>
-      <c r="E16" t="s">
-        <v>62</v>
       </c>
       <c r="F16">
         <v>2</v>
@@ -1059,16 +1059,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" t="s">
         <v>63</v>
-      </c>
-      <c r="C17" t="s">
-        <v>64</v>
-      </c>
-      <c r="D17" t="s">
-        <v>65</v>
-      </c>
-      <c r="E17" t="s">
-        <v>66</v>
       </c>
       <c r="F17">
         <v>1</v>
@@ -1082,16 +1082,16 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" t="s">
+        <v>65</v>
+      </c>
+      <c r="E18" t="s">
         <v>67</v>
-      </c>
-      <c r="C18" t="s">
-        <v>68</v>
-      </c>
-      <c r="D18" t="s">
-        <v>69</v>
-      </c>
-      <c r="E18" t="s">
-        <v>70</v>
       </c>
       <c r="F18">
         <v>4</v>
@@ -1105,16 +1105,16 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C19" t="s">
-        <v>72</v>
+        <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>4</v>
+        <v>69</v>
       </c>
       <c r="E19" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -1128,16 +1128,16 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E20" t="s">
         <v>74</v>
-      </c>
-      <c r="C20" t="s">
-        <v>75</v>
-      </c>
-      <c r="D20" t="s">
-        <v>76</v>
-      </c>
-      <c r="E20" t="s">
-        <v>77</v>
       </c>
       <c r="F20">
         <v>4</v>
@@ -1151,16 +1151,16 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C21" t="s">
+        <v>77</v>
+      </c>
+      <c r="D21" t="s">
+        <v>76</v>
+      </c>
+      <c r="E21" t="s">
         <v>78</v>
-      </c>
-      <c r="C21" t="s">
-        <v>79</v>
-      </c>
-      <c r="D21" t="s">
-        <v>80</v>
-      </c>
-      <c r="E21" t="s">
-        <v>81</v>
       </c>
       <c r="F21">
         <v>3</v>

</xml_diff>

<commit_message>
clean up old / unused stimuli
</commit_message>
<xml_diff>
--- a/material-vn/item_order.xlsx
+++ b/material-vn/item_order.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ameli\Desktop\Arbeit\orev-vn\material-vn\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliaprein/academiccloudsync/studies/orev-vn/public/material-vn/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F8E52462-CC6A-4ED0-9A56-026AFC9626C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E35FB9B-B0CD-A049-981F-6007DA32CD56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{9D79C90C-9F7D-2F46-9E4F-8B298AB5B9D9}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{9D79C90C-9F7D-2F46-9E4F-8B298AB5B9D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -339,7 +338,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -355,7 +354,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -673,21 +672,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{799C0DEA-28D9-6C42-8CEC-3504E277A21A}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" zoomScale="155" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.296875" customWidth="1"/>
-    <col min="2" max="2" width="13.69921875" customWidth="1"/>
-    <col min="3" max="3" width="24.69921875" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="24.19921875" customWidth="1"/>
+    <col min="5" max="5" width="24.1640625" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>81</v>
       </c>
@@ -710,7 +709,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -733,7 +732,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -756,7 +755,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -779,7 +778,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -802,7 +801,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -825,7 +824,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -848,7 +847,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -871,7 +870,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -894,7 +893,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -917,7 +916,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -940,7 +939,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -963,7 +962,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -986,7 +985,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1009,7 +1008,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1032,7 +1031,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1055,7 +1054,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1078,7 +1077,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1101,7 +1100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1124,7 +1123,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1147,7 +1146,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>

</xml_diff>